<commit_message>
batch-yaml..py, claude-fix..yaml both working, eb accepts lim necessary only fields, model now returning text string, still working on yaml to return full structured csv line per listing
</commit_message>
<xml_diff>
--- a/archives-all/ebay-auto-listings-2gents-SacTree-GawainGreen.xlsx
+++ b/archives-all/ebay-auto-listings-2gents-SacTree-GawainGreen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\dev\projects\ebay-posting-automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\dev\projects\ebay-posting-automation\archives-all\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45AA7E7D-E6A7-4E70-8D4E-54760E4CBB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8474955-F8F0-4AAB-868B-E2A185FE8A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="0" windowWidth="24285" windowHeight="9615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listings" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>*Action(SiteID=US|Country=US|Currency=USD|Version=1193)</t>
   </si>
@@ -322,39 +322,6 @@
   </si>
   <si>
     <t>English</t>
-  </si>
-  <si>
-    <t>The Two Gentlemen of Verona (The Arden Shakespeare)</t>
-  </si>
-  <si>
-    <t>Condition Notes:
-Very Good in Good+ jacket: blue cloth boards bright; binding square and tight; pages clean with only faint toning to edges. Jacket retains colour, light edge-rubs, small chip at head of spine and faint splash mark to lower rear panel, now in removable archival sleeve.
-Collector Details:
-Bibliographic Details
-- Author: William Shakespeare
-- Title: The Two Gentlemen of Verona
-- Editor: Clifford Leech (Arden Second Series)
-- Publisher / Place: Methuen &amp; Co. Ltd., London
-- Year: 1969
-- Edition / Printing: First printing of the completely revised &amp; reset edition (first thus for Leech text; previous Arden issue 1906 by Warwick Bond)
-- Format: Crown 8vo hardcover; li + 188 pp. including Introduction, Text, Commentary &amp; Index
-- Binding Details: Original blue cloth; gilt spine lettering; publisher's blind colophon to upper board
-- Dust Jacket: Printed teal/white jacket with decorative border; priced; now protected in Mylar
-- Notable Points: Includes comprehensive introduction on sources, date, stage history; full textual notes; SBN 416 47490 X
-- Language: English
-Condition (conservative, ABAA-style)
-- Boards/Spine: Clean cloth, minor rubbing to extremities, bright gilt
-- Pages/Textblock: Creamy pages, firm; no writing or marks noted
-- Hinges/Binding: Tight, square; no cracking
-- Edges: Very slight dusting to top edge
-- Dust Jacket: Edge-wear with short closed tears, nick at spine crown, faint rear panel staining; colors strong, unclipped
-- Overall grade: Very Good book / Good+ jacket</t>
-  </si>
-  <si>
-    <t>William Shakespeare</t>
-  </si>
-  <si>
-    <t>The Sacred Tree: Being the Second Part of ‘The Tale of Genji'</t>
   </si>
   <si>
     <t>Collector Details:
@@ -364,31 +331,16 @@
     <t>Lady Murasaki (Murasaki Shikibu); translated by Arthur Waley</t>
   </si>
   <si>
-    <t>Pearl; Sir Gawain and the Green Knight</t>
-  </si>
-  <si>
-    <t>Condition Notes:
-Good+. Clean brown cloth a little rubbed with a surface scratch to upper board, mild fray to spine foot &amp; a corner; gilt spine titling bright. Page edges evenly toned, one small smudge to lower edge. EL endpapers show owner's pencilled &amp; inked notes. Tight, square binding; text clean with only scattered faint handling.
-Collector Details:
-['Bibliographic Details', 'Author: Anonymous (‘Pearl' / ‘Gawain' Poet); Editor &amp; Introduction: A. C. Cawley', 'Title: Pearl; Sir Gawain and the Green Knight', 'Publisher / Place: J. M. Dent &amp; Sons Ltd., Aldine House, Bedford St., London | Co-issue: E. P. Dutton &amp; Co., New York', 'Year: 1966 (copyright 1962; statement: ‘Last reprinted 1966')', 'Edition / Printing: Everyman's Library No. 346, 1966 Reprint', 'Format: Crown 8vo hardcover; approx. xxxii + 204 pp.', 'Binding Details: Original brown cloth; double gilt rules at crown; gilt titling &amp; EL script monogram to spine; EL anchor-monogram patterned endpapers', 'Dust Jacket: Not present (often lost)', 'Notable Points: Full Middle English text with scholarly apparatus; glossary, textual notes, bibliographical check-list', 'Language: English (Middle English text with modern English notes)', 'Condition (conservative, ABAA-style)', 'Boards/Spine: Light rubbing; surface scratch to upper board; mild corner &amp; spine-end wear; gilt bright.', 'Pages/Textblock: Clean, evenly toned stock; a few faint handling marks; no underlining in text.', 'Endpapers: EL pattern; previous owner's ink annotations on front &amp; rear pastedowns.', 'Hinges/Binding: Firm and square; no loose leaves.', 'Edges: Toned; one small spot to lower edge.', 'Overall grade: Good+ (solid reading / reference copy in original cloth).']</t>
-  </si>
-  <si>
-    <t>Anonymous (The Pearl / Gawain Poet); edited with introduction by A. C. Cawley, M.A., Ph.D.</t>
-  </si>
-  <si>
     <t>Generated</t>
   </si>
   <si>
     <t>2025-10-13T20:16:44</t>
   </si>
   <si>
-    <t>https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-01.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-02.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-03.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-04.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-05.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-06.jpg</t>
-  </si>
-  <si>
     <t>https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-01.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-02.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-03.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-04.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-05.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-06.jpg</t>
   </si>
   <si>
-    <t>https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-01.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-02.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-03.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-04.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-05.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-06.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-07.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-08.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-09.jpg</t>
+    <t>The Sacred Tree, Vol. 2: ‘The Tale of Genji'</t>
   </si>
 </sst>
 </file>
@@ -764,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE9"/>
+  <dimension ref="A1:CE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K5"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,22 +991,22 @@
         <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="K2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="O2" t="s">
         <v>86</v>
       </c>
       <c r="P2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q2" t="s">
         <v>87</v>
@@ -1075,131 +1027,16 @@
         <v>92</v>
       </c>
       <c r="AM2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AO2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3">
-        <v>100</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>106</v>
-      </c>
-      <c r="O3" t="s">
-        <v>86</v>
-      </c>
-      <c r="P3" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>87</v>
-      </c>
-      <c r="R3" t="s">
-        <v>88</v>
-      </c>
-      <c r="X3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" t="s">
-        <v>100</v>
-      </c>
-      <c r="K4">
-        <v>100</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>107</v>
-      </c>
-      <c r="O4" t="s">
-        <v>86</v>
-      </c>
-      <c r="P4" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>87</v>
-      </c>
-      <c r="R4" t="s">
-        <v>88</v>
-      </c>
-      <c r="X4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>100</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="AZ9">
-        <f>LEN(AZ4)</f>
-        <v>0</v>
+    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="AZ7" t="e">
+        <f>LEN(#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -1217,10 +1054,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>